<commit_message>
updated input spreadsheet based on planned weighted selection and minimum item numbers from a category
</commit_message>
<xml_diff>
--- a/practice_elements.xlsx
+++ b/practice_elements.xlsx
@@ -7,14 +7,19 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="items" sheetId="1" r:id="rId1"/>
+    <sheet name="categories" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">categories!$A$1:$B$1</definedName>
+    <definedName name="categories">categories!$A$2:$A$10</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -31,9 +36,6 @@
     <t>pattern</t>
   </si>
   <si>
-    <t>priority</t>
-  </si>
-  <si>
     <t>technique</t>
   </si>
   <si>
@@ -83,6 +85,27 @@
   </si>
   <si>
     <t>must do first</t>
+  </si>
+  <si>
+    <t>sort_order</t>
+  </si>
+  <si>
+    <t>min_items</t>
+  </si>
+  <si>
+    <t>explore</t>
+  </si>
+  <si>
+    <t>e1</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>e2</t>
+  </si>
+  <si>
+    <t>r2</t>
   </si>
 </sst>
 </file>
@@ -433,18 +456,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,15 +482,18 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -483,10 +510,13 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -503,10 +533,13 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -523,10 +556,13 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -543,10 +579,13 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -563,16 +602,19 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -583,93 +625,108 @@
       <c r="F7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -678,53 +735,205 @@
         <v>10</v>
       </c>
       <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15">
         <v>3</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576 B1">
+      <formula1>categories</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>5</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added support for weighted selection
</commit_message>
<xml_diff>
--- a/practice_elements.xlsx
+++ b/practice_elements.xlsx
@@ -459,7 +459,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,16 +499,16 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -522,10 +522,10 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -545,10 +545,10 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -568,10 +568,10 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -591,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -603,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -614,10 +614,10 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -637,10 +637,10 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -660,10 +660,10 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -683,10 +683,10 @@
         <v>5</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -706,10 +706,10 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -729,13 +729,13 @@
         <v>17</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>10</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -804,13 +804,13 @@
         <v>10</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -821,19 +821,19 @@
         <v>24</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -847,7 +847,7 @@
         <v>5</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E17">
         <v>3</v>

</xml_diff>

<commit_message>
implemented min item counts per category. improved handling of session time filling
</commit_message>
<xml_diff>
--- a/practice_elements.xlsx
+++ b/practice_elements.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,13 +15,14 @@
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">categories!$A$1:$B$1</definedName>
     <definedName function="false" hidden="false" name="categories" vbProcedure="false">categories!$A$2:$A$10</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">categories!$A$1:$B$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">categories!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -105,6 +106,9 @@
   </si>
   <si>
     <t>r2</t>
+  </si>
+  <si>
+    <t>e3</t>
   </si>
   <si>
     <t>min_items</t>
@@ -194,12 +198,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -224,10 +232,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -264,7 +272,7 @@
       <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="0" t="n">
@@ -287,7 +295,7 @@
       <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -310,7 +318,7 @@
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -333,7 +341,7 @@
       <c r="A5" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="0" t="n">
@@ -356,7 +364,7 @@
       <c r="A6" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -379,7 +387,7 @@
       <c r="A7" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -402,11 +410,11 @@
       <c r="A8" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>3</v>
@@ -425,11 +433,11 @@
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>3</v>
@@ -448,11 +456,11 @@
       <c r="A10" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>3</v>
@@ -471,11 +479,11 @@
       <c r="A11" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>3</v>
@@ -494,7 +502,7 @@
       <c r="A12" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="0" t="n">
@@ -517,7 +525,7 @@
       <c r="A13" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="0" t="n">
@@ -540,7 +548,7 @@
       <c r="A14" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="0" t="n">
@@ -563,7 +571,7 @@
       <c r="A15" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="0" t="n">
@@ -586,7 +594,7 @@
       <c r="A16" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="0" t="n">
@@ -609,7 +617,7 @@
       <c r="A17" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="0" t="n">
@@ -625,6 +633,29 @@
         <v>0</v>
       </c>
       <c r="G17" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -652,7 +683,7 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -668,20 +699,26 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>14</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
implemented max item limits per category
</commit_message>
<xml_diff>
--- a/practice_elements.xlsx
+++ b/practice_elements.xlsx
@@ -235,7 +235,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -276,10 +276,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>2</v>
@@ -299,10 +299,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>2</v>
@@ -322,10 +322,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>2</v>
@@ -345,10 +345,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>2</v>
@@ -368,10 +368,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>2</v>
@@ -391,7 +391,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>3</v>
@@ -506,7 +506,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>10</v>
@@ -532,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>2</v>
@@ -555,7 +555,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>2</v>
@@ -624,7 +624,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>3</v>
@@ -684,7 +684,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -709,9 +709,6 @@
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -721,28 +718,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>1</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
adding support for item time scaling
</commit_message>
<xml_diff>
--- a/practice_elements.xlsx
+++ b/practice_elements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\col52j\Documents\Code\practice-randomiser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2FED73E3-0E21-47D3-B86C-10BE50B964DF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9A07CE90-15F7-4084-B3CE-D847C72A6734}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -504,7 +504,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,10 +834,10 @@
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
         <v>5</v>
-      </c>
-      <c r="F13">
-        <v>10</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -859,10 +859,10 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
         <v>5</v>
-      </c>
-      <c r="F14">
-        <v>10</v>
       </c>
       <c r="G14">
         <v>2</v>

</xml_diff>

<commit_message>
updating time scaling so it is adjustable per-category via a metadata column 'scale_time'
</commit_message>
<xml_diff>
--- a/practice_elements.xlsx
+++ b/practice_elements.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t xml:space="preserve">max_items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scale_time</t>
   </si>
 </sst>
 </file>
@@ -757,10 +760,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -780,10 +783,16 @@
       <c r="C1" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -793,6 +802,9 @@
       <c r="B3" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -801,6 +813,9 @@
       <c r="C4" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -812,6 +827,9 @@
       <c r="C5" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -819,6 +837,9 @@
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>